<commit_message>
Added etron,z06,zr1, taycan, brz, all teslas
</commit_message>
<xml_diff>
--- a/Price_Puller.xlsx
+++ b/Price_Puller.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\derek\Dropbox (Personal)\Cars\Price Puller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\derek\Dropbox (Personal)\Cars\Price Puller Used Cars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D23BD84-0E55-477C-AAE2-2E4AFE33AFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBA031E-723A-4537-B4E9-CD9DE5BB4D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-2750" windowWidth="38620" windowHeight="21220" tabRatio="831" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="-2750" windowWidth="38620" windowHeight="21220" tabRatio="977" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Q5" sheetId="1" r:id="rId1"/>
@@ -18,37 +18,44 @@
     <sheet name="RS4" sheetId="3" r:id="rId3"/>
     <sheet name="RS7" sheetId="4" r:id="rId4"/>
     <sheet name="S4" sheetId="5" r:id="rId5"/>
-    <sheet name="M3" sheetId="6" r:id="rId6"/>
-    <sheet name="M5" sheetId="7" r:id="rId7"/>
-    <sheet name="Corvette" sheetId="8" r:id="rId8"/>
-    <sheet name="458 Italia" sheetId="9" r:id="rId9"/>
-    <sheet name="F250" sheetId="10" r:id="rId10"/>
-    <sheet name="GT" sheetId="11" r:id="rId11"/>
-    <sheet name="S2000" sheetId="12" r:id="rId12"/>
-    <sheet name="Wrangler" sheetId="13" r:id="rId13"/>
-    <sheet name="Aventador" sheetId="14" r:id="rId14"/>
-    <sheet name="Gallardo" sheetId="15" r:id="rId15"/>
-    <sheet name="Huracan" sheetId="16" r:id="rId16"/>
-    <sheet name="Murcielago" sheetId="17" r:id="rId17"/>
-    <sheet name="Urus" sheetId="18" r:id="rId18"/>
-    <sheet name="AMG" sheetId="19" r:id="rId19"/>
-    <sheet name="C63 AMG" sheetId="20" r:id="rId20"/>
-    <sheet name="Carrera S" sheetId="21" r:id="rId21"/>
-    <sheet name="GT3" sheetId="22" r:id="rId22"/>
-    <sheet name="GT3RS" sheetId="23" r:id="rId23"/>
-    <sheet name="GT4" sheetId="24" r:id="rId24"/>
-    <sheet name="GT4RS" sheetId="25" r:id="rId25"/>
-    <sheet name="Cayenne" sheetId="26" r:id="rId26"/>
-    <sheet name="Macan" sheetId="27" r:id="rId27"/>
-    <sheet name="Model 3" sheetId="28" r:id="rId28"/>
-    <sheet name="Model X" sheetId="29" r:id="rId29"/>
+    <sheet name="Etron" sheetId="30" r:id="rId6"/>
+    <sheet name="M3" sheetId="6" r:id="rId7"/>
+    <sheet name="M5" sheetId="7" r:id="rId8"/>
+    <sheet name="Corvette Z06" sheetId="31" r:id="rId9"/>
+    <sheet name="Corvette ZR1" sheetId="32" r:id="rId10"/>
+    <sheet name="458 Italia" sheetId="9" r:id="rId11"/>
+    <sheet name="F250" sheetId="10" r:id="rId12"/>
+    <sheet name="GT" sheetId="11" r:id="rId13"/>
+    <sheet name="S2000" sheetId="12" r:id="rId14"/>
+    <sheet name="Wrangler" sheetId="13" r:id="rId15"/>
+    <sheet name="Aventador" sheetId="14" r:id="rId16"/>
+    <sheet name="Gallardo" sheetId="15" r:id="rId17"/>
+    <sheet name="Huracan" sheetId="16" r:id="rId18"/>
+    <sheet name="Murcielago" sheetId="17" r:id="rId19"/>
+    <sheet name="Urus" sheetId="18" r:id="rId20"/>
+    <sheet name="AMG" sheetId="19" r:id="rId21"/>
+    <sheet name="C63 AMG" sheetId="20" r:id="rId22"/>
+    <sheet name="Carrera S" sheetId="21" r:id="rId23"/>
+    <sheet name="GT3" sheetId="22" r:id="rId24"/>
+    <sheet name="GT3RS" sheetId="23" r:id="rId25"/>
+    <sheet name="GT4" sheetId="24" r:id="rId26"/>
+    <sheet name="GT4RS" sheetId="25" r:id="rId27"/>
+    <sheet name="Cayenne" sheetId="26" r:id="rId28"/>
+    <sheet name="Macan" sheetId="27" r:id="rId29"/>
+    <sheet name="Taycan" sheetId="33" r:id="rId30"/>
+    <sheet name="BRZ" sheetId="34" r:id="rId31"/>
+    <sheet name="Model 3" sheetId="28" r:id="rId32"/>
+    <sheet name="Model X" sheetId="29" r:id="rId33"/>
+    <sheet name="CyberTruck" sheetId="35" r:id="rId34"/>
+    <sheet name="Model Y" sheetId="36" r:id="rId35"/>
+    <sheet name="Model S" sheetId="37" r:id="rId36"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -57,6 +64,12 @@
   </si>
   <si>
     <t>24APR2025</t>
+  </si>
+  <si>
+    <t>25APR2025</t>
+  </si>
+  <si>
+    <t>26APR2025</t>
   </si>
   <si>
     <t>22APR2025</t>
@@ -69,7 +82,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +98,11 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -131,6 +149,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,7 +452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
@@ -568,14 +587,295 @@
         <v>57255</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>11302</v>
+      </c>
+      <c r="C5" s="4">
+        <v>12586</v>
+      </c>
+      <c r="D5" s="4">
+        <v>13274</v>
+      </c>
+      <c r="E5" s="4">
+        <v>15062</v>
+      </c>
+      <c r="F5" s="4">
+        <v>18281</v>
+      </c>
+      <c r="G5" s="4">
+        <v>21192</v>
+      </c>
+      <c r="H5" s="4">
+        <v>24323</v>
+      </c>
+      <c r="I5" s="4">
+        <v>27947</v>
+      </c>
+      <c r="J5" s="4">
+        <v>32306</v>
+      </c>
+      <c r="K5" s="4">
+        <v>33249</v>
+      </c>
+      <c r="L5" s="4">
+        <v>45910</v>
+      </c>
+      <c r="M5" s="4">
+        <v>57227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>11424</v>
+      </c>
+      <c r="C6" s="4">
+        <v>12597</v>
+      </c>
+      <c r="D6" s="4">
+        <v>13305</v>
+      </c>
+      <c r="E6" s="4">
+        <v>15056</v>
+      </c>
+      <c r="F6" s="4">
+        <v>18269</v>
+      </c>
+      <c r="G6" s="4">
+        <v>21174</v>
+      </c>
+      <c r="H6" s="4">
+        <v>24182</v>
+      </c>
+      <c r="I6" s="4">
+        <v>27928</v>
+      </c>
+      <c r="J6" s="4">
+        <v>32294</v>
+      </c>
+      <c r="K6" s="4">
+        <v>33190</v>
+      </c>
+      <c r="L6" s="4">
+        <v>45882</v>
+      </c>
+      <c r="M6" s="4">
+        <v>57264</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6">
+        <v>1992</v>
+      </c>
+      <c r="C1" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D1" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E1" s="6">
+        <v>2011</v>
+      </c>
+      <c r="F1" s="6">
+        <v>2012</v>
+      </c>
+      <c r="G1" s="6">
+        <v>2013</v>
+      </c>
+      <c r="H1" s="6">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>36500</v>
+      </c>
+      <c r="C6" s="4">
+        <v>97785</v>
+      </c>
+      <c r="D6" s="4">
+        <v>91712</v>
+      </c>
+      <c r="E6" s="4">
+        <v>97890</v>
+      </c>
+      <c r="F6" s="4">
+        <v>92948</v>
+      </c>
+      <c r="G6" s="4">
+        <v>104999</v>
+      </c>
+      <c r="H6" s="4">
+        <v>202447</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5">
+        <v>2010</v>
+      </c>
+      <c r="C1" s="5">
+        <v>2011</v>
+      </c>
+      <c r="D1" s="5">
+        <v>2012</v>
+      </c>
+      <c r="E1" s="5">
+        <v>2013</v>
+      </c>
+      <c r="F1" s="5">
+        <v>2014</v>
+      </c>
+      <c r="G1" s="5">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>194782</v>
+      </c>
+      <c r="C3" s="4">
+        <v>201635</v>
+      </c>
+      <c r="D3" s="4">
+        <v>204811</v>
+      </c>
+      <c r="E3" s="4">
+        <v>213776</v>
+      </c>
+      <c r="F3" s="4">
+        <v>249238</v>
+      </c>
+      <c r="G3" s="4">
+        <v>221576</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>195060</v>
+      </c>
+      <c r="C4" s="4">
+        <v>204060</v>
+      </c>
+      <c r="D4" s="4">
+        <v>204478</v>
+      </c>
+      <c r="E4" s="4">
+        <v>213776</v>
+      </c>
+      <c r="F4" s="4">
+        <v>249238</v>
+      </c>
+      <c r="G4" s="4">
+        <v>221576</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>195060</v>
+      </c>
+      <c r="C5" s="4">
+        <v>204852</v>
+      </c>
+      <c r="D5" s="4">
+        <v>204478</v>
+      </c>
+      <c r="E5" s="4">
+        <v>213776</v>
+      </c>
+      <c r="F5" s="4">
+        <v>249238</v>
+      </c>
+      <c r="G5" s="4">
+        <v>221576</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>194292</v>
+      </c>
+      <c r="C6" s="4">
+        <v>207698</v>
+      </c>
+      <c r="D6" s="4">
+        <v>204478</v>
+      </c>
+      <c r="E6" s="4">
+        <v>213776</v>
+      </c>
+      <c r="F6" s="4">
+        <v>249238</v>
+      </c>
+      <c r="G6" s="4">
+        <v>221576</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I47" sqref="I47"/>
@@ -710,14 +1010,96 @@
         <v>74584</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>24726</v>
+      </c>
+      <c r="C5" s="4">
+        <v>25788</v>
+      </c>
+      <c r="D5" s="4">
+        <v>28854</v>
+      </c>
+      <c r="E5" s="4">
+        <v>36467</v>
+      </c>
+      <c r="F5" s="4">
+        <v>38400</v>
+      </c>
+      <c r="G5" s="4">
+        <v>40742</v>
+      </c>
+      <c r="H5" s="4">
+        <v>46151</v>
+      </c>
+      <c r="I5" s="4">
+        <v>51556</v>
+      </c>
+      <c r="J5" s="4">
+        <v>54513</v>
+      </c>
+      <c r="K5" s="4">
+        <v>63550</v>
+      </c>
+      <c r="L5" s="4">
+        <v>69439</v>
+      </c>
+      <c r="M5" s="4">
+        <v>74564</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>24613</v>
+      </c>
+      <c r="C6" s="4">
+        <v>25798</v>
+      </c>
+      <c r="D6" s="4">
+        <v>28820</v>
+      </c>
+      <c r="E6" s="4">
+        <v>36416</v>
+      </c>
+      <c r="F6" s="4">
+        <v>38313</v>
+      </c>
+      <c r="G6" s="4">
+        <v>40948</v>
+      </c>
+      <c r="H6" s="4">
+        <v>46193</v>
+      </c>
+      <c r="I6" s="4">
+        <v>51618</v>
+      </c>
+      <c r="J6" s="4">
+        <v>54603</v>
+      </c>
+      <c r="K6" s="4">
+        <v>63428</v>
+      </c>
+      <c r="L6" s="4">
+        <v>69368</v>
+      </c>
+      <c r="M6" s="4">
+        <v>74557</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:G3"/>
@@ -799,14 +1181,60 @@
         <v>1172998</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>551626</v>
+      </c>
+      <c r="C5" s="4">
+        <v>598647</v>
+      </c>
+      <c r="D5" s="4">
+        <v>883647</v>
+      </c>
+      <c r="E5" s="4">
+        <v>922827</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1274995</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1172998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>553348</v>
+      </c>
+      <c r="C6" s="4">
+        <v>598647</v>
+      </c>
+      <c r="D6" s="4">
+        <v>883647</v>
+      </c>
+      <c r="E6" s="4">
+        <v>922826</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1274995</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1172998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
@@ -914,14 +1342,78 @@
         <v>47049</v>
       </c>
     </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>29872</v>
+      </c>
+      <c r="C5" s="4">
+        <v>28549</v>
+      </c>
+      <c r="D5" s="4">
+        <v>24863</v>
+      </c>
+      <c r="E5" s="4">
+        <v>26236</v>
+      </c>
+      <c r="F5" s="4">
+        <v>31493</v>
+      </c>
+      <c r="G5" s="4">
+        <v>32648</v>
+      </c>
+      <c r="H5" s="4">
+        <v>32956</v>
+      </c>
+      <c r="I5" s="4">
+        <v>33217</v>
+      </c>
+      <c r="J5" s="4">
+        <v>49117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>30112</v>
+      </c>
+      <c r="C6" s="4">
+        <v>28322</v>
+      </c>
+      <c r="D6" s="4">
+        <v>24863</v>
+      </c>
+      <c r="E6" s="4">
+        <v>26760</v>
+      </c>
+      <c r="F6" s="4">
+        <v>32185</v>
+      </c>
+      <c r="G6" s="4">
+        <v>33223</v>
+      </c>
+      <c r="H6" s="4">
+        <v>32638</v>
+      </c>
+      <c r="I6" s="4">
+        <v>33217</v>
+      </c>
+      <c r="J6" s="4">
+        <v>49117</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:M3"/>
@@ -1056,14 +1548,96 @@
         <v>52293</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>17953</v>
+      </c>
+      <c r="C5" s="4">
+        <v>18975</v>
+      </c>
+      <c r="D5" s="4">
+        <v>20343</v>
+      </c>
+      <c r="E5" s="4">
+        <v>22279</v>
+      </c>
+      <c r="F5" s="4">
+        <v>25141</v>
+      </c>
+      <c r="G5" s="4">
+        <v>28244</v>
+      </c>
+      <c r="H5" s="4">
+        <v>29959</v>
+      </c>
+      <c r="I5" s="4">
+        <v>32838</v>
+      </c>
+      <c r="J5" s="4">
+        <v>36068</v>
+      </c>
+      <c r="K5" s="4">
+        <v>38911</v>
+      </c>
+      <c r="L5" s="4">
+        <v>51639</v>
+      </c>
+      <c r="M5" s="4">
+        <v>52325</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>17946</v>
+      </c>
+      <c r="C6" s="4">
+        <v>18992</v>
+      </c>
+      <c r="D6" s="4">
+        <v>20329</v>
+      </c>
+      <c r="E6" s="4">
+        <v>22295</v>
+      </c>
+      <c r="F6" s="4">
+        <v>25133</v>
+      </c>
+      <c r="G6" s="4">
+        <v>28283</v>
+      </c>
+      <c r="H6" s="4">
+        <v>29983</v>
+      </c>
+      <c r="I6" s="4">
+        <v>32856</v>
+      </c>
+      <c r="J6" s="4">
+        <v>36034</v>
+      </c>
+      <c r="K6" s="4">
+        <v>38901</v>
+      </c>
+      <c r="L6" s="4">
+        <v>51651</v>
+      </c>
+      <c r="M6" s="4">
+        <v>52345</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:L3"/>
@@ -1191,14 +1765,90 @@
         <v>976629</v>
       </c>
     </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>313913</v>
+      </c>
+      <c r="C5" s="4">
+        <v>304754</v>
+      </c>
+      <c r="D5" s="4">
+        <v>346455</v>
+      </c>
+      <c r="E5" s="4">
+        <v>364186</v>
+      </c>
+      <c r="F5" s="4">
+        <v>369808</v>
+      </c>
+      <c r="G5" s="4">
+        <v>520317</v>
+      </c>
+      <c r="H5" s="4">
+        <v>411202</v>
+      </c>
+      <c r="I5" s="4">
+        <v>598857</v>
+      </c>
+      <c r="J5" s="4">
+        <v>756119</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1030400</v>
+      </c>
+      <c r="L5" s="4">
+        <v>979754</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>306699</v>
+      </c>
+      <c r="C6" s="4">
+        <v>292052</v>
+      </c>
+      <c r="D6" s="4">
+        <v>346455</v>
+      </c>
+      <c r="E6" s="4">
+        <v>364186</v>
+      </c>
+      <c r="F6" s="4">
+        <v>366601</v>
+      </c>
+      <c r="G6" s="4">
+        <v>520317</v>
+      </c>
+      <c r="H6" s="4">
+        <v>421281</v>
+      </c>
+      <c r="I6" s="4">
+        <v>593708</v>
+      </c>
+      <c r="J6" s="4">
+        <v>780353</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1003378</v>
+      </c>
+      <c r="L6" s="4">
+        <v>962704</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:K3"/>
@@ -1316,14 +1966,84 @@
         <v>128695</v>
       </c>
     </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>96557</v>
+      </c>
+      <c r="C5" s="4">
+        <v>125558</v>
+      </c>
+      <c r="D5" s="4">
+        <v>103736</v>
+      </c>
+      <c r="E5" s="4">
+        <v>104998</v>
+      </c>
+      <c r="F5" s="4">
+        <v>167838</v>
+      </c>
+      <c r="G5" s="4">
+        <v>122995</v>
+      </c>
+      <c r="H5" s="4">
+        <v>135498</v>
+      </c>
+      <c r="I5" s="4">
+        <v>156555</v>
+      </c>
+      <c r="J5" s="4">
+        <v>154245</v>
+      </c>
+      <c r="K5" s="4">
+        <v>128695</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>96497</v>
+      </c>
+      <c r="C6" s="4">
+        <v>131296</v>
+      </c>
+      <c r="D6" s="4">
+        <v>103736</v>
+      </c>
+      <c r="E6" s="4">
+        <v>104998</v>
+      </c>
+      <c r="F6" s="4">
+        <v>167838</v>
+      </c>
+      <c r="G6" s="4">
+        <v>120996</v>
+      </c>
+      <c r="H6" s="4">
+        <v>135498</v>
+      </c>
+      <c r="I6" s="4">
+        <v>156555</v>
+      </c>
+      <c r="J6" s="4">
+        <v>154245</v>
+      </c>
+      <c r="K6" s="4">
+        <v>128695</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:K3"/>
@@ -1440,14 +2160,84 @@
         <v>340813</v>
       </c>
     </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>200507</v>
+      </c>
+      <c r="C5" s="4">
+        <v>222941</v>
+      </c>
+      <c r="D5" s="4">
+        <v>207342</v>
+      </c>
+      <c r="E5" s="4">
+        <v>303094</v>
+      </c>
+      <c r="F5" s="4">
+        <v>279194</v>
+      </c>
+      <c r="G5" s="4">
+        <v>269156</v>
+      </c>
+      <c r="H5" s="4">
+        <v>279989</v>
+      </c>
+      <c r="I5" s="4">
+        <v>330966</v>
+      </c>
+      <c r="J5" s="4">
+        <v>343632</v>
+      </c>
+      <c r="K5" s="4">
+        <v>342109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>200507</v>
+      </c>
+      <c r="C6" s="4">
+        <v>222444</v>
+      </c>
+      <c r="D6" s="4">
+        <v>207342</v>
+      </c>
+      <c r="E6" s="4">
+        <v>300391</v>
+      </c>
+      <c r="F6" s="4">
+        <v>275241</v>
+      </c>
+      <c r="G6" s="4">
+        <v>268977</v>
+      </c>
+      <c r="H6" s="4">
+        <v>279726</v>
+      </c>
+      <c r="I6" s="4">
+        <v>328071</v>
+      </c>
+      <c r="J6" s="4">
+        <v>343624</v>
+      </c>
+      <c r="K6" s="4">
+        <v>341324</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:H3"/>
@@ -1538,14 +2328,291 @@
         <v>1146926</v>
       </c>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>404450</v>
+      </c>
+      <c r="C5" s="4">
+        <v>289665</v>
+      </c>
+      <c r="D5" s="4">
+        <v>471598</v>
+      </c>
+      <c r="E5" s="4">
+        <v>275766</v>
+      </c>
+      <c r="F5" s="4">
+        <v>349905</v>
+      </c>
+      <c r="G5" s="4">
+        <v>390000</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1146926</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>404450</v>
+      </c>
+      <c r="C6" s="4">
+        <v>289665</v>
+      </c>
+      <c r="D6" s="4">
+        <v>599898</v>
+      </c>
+      <c r="E6" s="4">
+        <v>275766</v>
+      </c>
+      <c r="F6" s="4">
+        <v>349905</v>
+      </c>
+      <c r="G6" s="4">
+        <v>390000</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1217540</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5">
+        <v>2008</v>
+      </c>
+      <c r="C1" s="5">
+        <v>2009</v>
+      </c>
+      <c r="D1" s="5">
+        <v>2011</v>
+      </c>
+      <c r="E1" s="5">
+        <v>2012</v>
+      </c>
+      <c r="F1" s="5">
+        <v>2014</v>
+      </c>
+      <c r="G1" s="5">
+        <v>2015</v>
+      </c>
+      <c r="H1" s="5">
+        <v>2017</v>
+      </c>
+      <c r="I1" s="5">
+        <v>2018</v>
+      </c>
+      <c r="J1" s="5">
+        <v>2020</v>
+      </c>
+      <c r="K1" s="5">
+        <v>2021</v>
+      </c>
+      <c r="L1" s="5">
+        <v>2022</v>
+      </c>
+      <c r="M1" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>74344</v>
+      </c>
+      <c r="C3" s="4">
+        <v>70085</v>
+      </c>
+      <c r="D3" s="4">
+        <v>88918</v>
+      </c>
+      <c r="E3" s="4">
+        <v>113777</v>
+      </c>
+      <c r="F3" s="4">
+        <v>102040</v>
+      </c>
+      <c r="G3" s="4">
+        <v>103736</v>
+      </c>
+      <c r="H3" s="4">
+        <v>149100</v>
+      </c>
+      <c r="I3" s="4">
+        <v>141629</v>
+      </c>
+      <c r="J3" s="4">
+        <v>176792</v>
+      </c>
+      <c r="K3" s="4">
+        <v>157100</v>
+      </c>
+      <c r="L3" s="4">
+        <v>165900</v>
+      </c>
+      <c r="M3" s="4">
+        <v>217183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>74183</v>
+      </c>
+      <c r="C4" s="4">
+        <v>71149</v>
+      </c>
+      <c r="D4" s="4">
+        <v>92711</v>
+      </c>
+      <c r="E4" s="4">
+        <v>113541</v>
+      </c>
+      <c r="F4" s="4">
+        <v>103078</v>
+      </c>
+      <c r="G4" s="4">
+        <v>105965</v>
+      </c>
+      <c r="H4" s="4">
+        <v>149100</v>
+      </c>
+      <c r="I4" s="4">
+        <v>143759</v>
+      </c>
+      <c r="J4" s="4">
+        <v>176487</v>
+      </c>
+      <c r="K4" s="4">
+        <v>157100</v>
+      </c>
+      <c r="L4" s="4">
+        <v>165816</v>
+      </c>
+      <c r="M4" s="4">
+        <v>218393</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>74183</v>
+      </c>
+      <c r="C5" s="4">
+        <v>71149</v>
+      </c>
+      <c r="D5" s="4">
+        <v>92511</v>
+      </c>
+      <c r="E5" s="4">
+        <v>113510</v>
+      </c>
+      <c r="F5" s="4">
+        <v>102902</v>
+      </c>
+      <c r="G5" s="4">
+        <v>105965</v>
+      </c>
+      <c r="H5" s="4">
+        <v>150145</v>
+      </c>
+      <c r="I5" s="4">
+        <v>140466</v>
+      </c>
+      <c r="J5" s="4">
+        <v>175516</v>
+      </c>
+      <c r="K5" s="4">
+        <v>156491</v>
+      </c>
+      <c r="L5" s="4">
+        <v>162258</v>
+      </c>
+      <c r="M5" s="4">
+        <v>216322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>74126</v>
+      </c>
+      <c r="C6" s="4">
+        <v>70691</v>
+      </c>
+      <c r="D6" s="4">
+        <v>92511</v>
+      </c>
+      <c r="E6" s="4">
+        <v>113510</v>
+      </c>
+      <c r="F6" s="4">
+        <v>104308</v>
+      </c>
+      <c r="G6" s="4">
+        <v>105965</v>
+      </c>
+      <c r="H6" s="4">
+        <v>150391</v>
+      </c>
+      <c r="I6" s="4">
+        <v>143560</v>
+      </c>
+      <c r="J6" s="4">
+        <v>175427</v>
+      </c>
+      <c r="K6" s="4">
+        <v>156158</v>
+      </c>
+      <c r="L6" s="4">
+        <v>162258</v>
+      </c>
+      <c r="M6" s="4">
+        <v>213239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
@@ -1626,14 +2693,60 @@
         <v>298049</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>175352</v>
+      </c>
+      <c r="C5" s="4">
+        <v>186788</v>
+      </c>
+      <c r="D5" s="4">
+        <v>203008</v>
+      </c>
+      <c r="E5" s="4">
+        <v>228551</v>
+      </c>
+      <c r="F5" s="4">
+        <v>272198</v>
+      </c>
+      <c r="G5" s="4">
+        <v>297087</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>175523</v>
+      </c>
+      <c r="C6" s="4">
+        <v>185897</v>
+      </c>
+      <c r="D6" s="4">
+        <v>202860</v>
+      </c>
+      <c r="E6" s="4">
+        <v>229301</v>
+      </c>
+      <c r="F6" s="4">
+        <v>271615</v>
+      </c>
+      <c r="G6" s="4">
+        <v>297585</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:I3"/>
@@ -1735,157 +2848,72 @@
         <v>168709</v>
       </c>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>72521</v>
+      </c>
+      <c r="C5" s="4">
+        <v>73291</v>
+      </c>
+      <c r="D5" s="4">
+        <v>105293</v>
+      </c>
+      <c r="E5" s="4">
+        <v>100810</v>
+      </c>
+      <c r="F5" s="4">
+        <v>139523</v>
+      </c>
+      <c r="G5" s="4">
+        <v>440611</v>
+      </c>
+      <c r="H5" s="4">
+        <v>157568</v>
+      </c>
+      <c r="I5" s="4">
+        <v>168650</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>72696</v>
+      </c>
+      <c r="C6" s="4">
+        <v>73342</v>
+      </c>
+      <c r="D6" s="4">
+        <v>105052</v>
+      </c>
+      <c r="E6" s="4">
+        <v>100810</v>
+      </c>
+      <c r="F6" s="4">
+        <v>139405</v>
+      </c>
+      <c r="G6" s="4">
+        <v>440611</v>
+      </c>
+      <c r="H6" s="4">
+        <v>157568</v>
+      </c>
+      <c r="I6" s="4">
+        <v>168610</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5">
-        <v>2008</v>
-      </c>
-      <c r="C1" s="5">
-        <v>2009</v>
-      </c>
-      <c r="D1" s="5">
-        <v>2011</v>
-      </c>
-      <c r="E1" s="5">
-        <v>2012</v>
-      </c>
-      <c r="F1" s="5">
-        <v>2014</v>
-      </c>
-      <c r="G1" s="5">
-        <v>2015</v>
-      </c>
-      <c r="H1" s="5">
-        <v>2017</v>
-      </c>
-      <c r="I1" s="5">
-        <v>2018</v>
-      </c>
-      <c r="J1" s="5">
-        <v>2020</v>
-      </c>
-      <c r="K1" s="5">
-        <v>2021</v>
-      </c>
-      <c r="L1" s="5">
-        <v>2022</v>
-      </c>
-      <c r="M1" s="5">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4">
-        <v>74344</v>
-      </c>
-      <c r="C3" s="4">
-        <v>70085</v>
-      </c>
-      <c r="D3" s="4">
-        <v>88918</v>
-      </c>
-      <c r="E3" s="4">
-        <v>113777</v>
-      </c>
-      <c r="F3" s="4">
-        <v>102040</v>
-      </c>
-      <c r="G3" s="4">
-        <v>103736</v>
-      </c>
-      <c r="H3" s="4">
-        <v>149100</v>
-      </c>
-      <c r="I3" s="4">
-        <v>141629</v>
-      </c>
-      <c r="J3" s="4">
-        <v>176792</v>
-      </c>
-      <c r="K3" s="4">
-        <v>157100</v>
-      </c>
-      <c r="L3" s="4">
-        <v>165900</v>
-      </c>
-      <c r="M3" s="4">
-        <v>217183</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4">
-        <v>74183</v>
-      </c>
-      <c r="C4" s="4">
-        <v>71149</v>
-      </c>
-      <c r="D4" s="4">
-        <v>92711</v>
-      </c>
-      <c r="E4" s="4">
-        <v>113541</v>
-      </c>
-      <c r="F4" s="4">
-        <v>103078</v>
-      </c>
-      <c r="G4" s="4">
-        <v>105965</v>
-      </c>
-      <c r="H4" s="4">
-        <v>149100</v>
-      </c>
-      <c r="I4" s="4">
-        <v>143759</v>
-      </c>
-      <c r="J4" s="4">
-        <v>176487</v>
-      </c>
-      <c r="K4" s="4">
-        <v>157100</v>
-      </c>
-      <c r="L4" s="4">
-        <v>165816</v>
-      </c>
-      <c r="M4" s="4">
-        <v>218393</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:M3"/>
@@ -2020,14 +3048,96 @@
         <v>99259</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>67693</v>
+      </c>
+      <c r="C5" s="4">
+        <v>35860</v>
+      </c>
+      <c r="D5" s="4">
+        <v>40439</v>
+      </c>
+      <c r="E5" s="4">
+        <v>33898</v>
+      </c>
+      <c r="F5" s="4">
+        <v>43305</v>
+      </c>
+      <c r="G5" s="4">
+        <v>46685</v>
+      </c>
+      <c r="H5" s="4">
+        <v>49939</v>
+      </c>
+      <c r="I5" s="4">
+        <v>57770</v>
+      </c>
+      <c r="J5" s="4">
+        <v>61036</v>
+      </c>
+      <c r="K5" s="4">
+        <v>82382</v>
+      </c>
+      <c r="L5" s="4">
+        <v>89391</v>
+      </c>
+      <c r="M5" s="4">
+        <v>99259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>67211</v>
+      </c>
+      <c r="C6" s="4">
+        <v>35849</v>
+      </c>
+      <c r="D6" s="4">
+        <v>38823</v>
+      </c>
+      <c r="E6" s="4">
+        <v>33876</v>
+      </c>
+      <c r="F6" s="4">
+        <v>43624</v>
+      </c>
+      <c r="G6" s="4">
+        <v>46978</v>
+      </c>
+      <c r="H6" s="4">
+        <v>49904</v>
+      </c>
+      <c r="I6" s="4">
+        <v>57879</v>
+      </c>
+      <c r="J6" s="4">
+        <v>60629</v>
+      </c>
+      <c r="K6" s="4">
+        <v>82420</v>
+      </c>
+      <c r="L6" s="4">
+        <v>89389</v>
+      </c>
+      <c r="M6" s="4">
+        <v>99178</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
@@ -2160,17 +3270,96 @@
         <v>179064</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>52104</v>
+      </c>
+      <c r="C5" s="4">
+        <v>56503</v>
+      </c>
+      <c r="D5" s="4">
+        <v>61233</v>
+      </c>
+      <c r="E5" s="4">
+        <v>70801</v>
+      </c>
+      <c r="F5" s="4">
+        <v>76900</v>
+      </c>
+      <c r="G5" s="4">
+        <v>74417</v>
+      </c>
+      <c r="I5" s="4">
+        <v>126373</v>
+      </c>
+      <c r="J5" s="4">
+        <v>135192</v>
+      </c>
+      <c r="K5" s="4">
+        <v>151686</v>
+      </c>
+      <c r="L5" s="4">
+        <v>160044</v>
+      </c>
+      <c r="M5" s="4">
+        <v>179357</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>52189</v>
+      </c>
+      <c r="C6" s="4">
+        <v>56453</v>
+      </c>
+      <c r="D6" s="4">
+        <v>61602</v>
+      </c>
+      <c r="E6" s="4">
+        <v>71141</v>
+      </c>
+      <c r="F6" s="4">
+        <v>78210</v>
+      </c>
+      <c r="G6" s="4">
+        <v>72836</v>
+      </c>
+      <c r="H6" s="4">
+        <v>104707</v>
+      </c>
+      <c r="I6" s="4">
+        <v>125220</v>
+      </c>
+      <c r="J6" s="4">
+        <v>134578</v>
+      </c>
+      <c r="K6" s="4">
+        <v>151396</v>
+      </c>
+      <c r="L6" s="4">
+        <v>159942</v>
+      </c>
+      <c r="M6" s="4">
+        <v>179664</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S50" sqref="S50"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,7 +3422,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3">
         <v>136544</v>
@@ -2352,6 +3541,88 @@
       </c>
       <c r="M4" s="4">
         <v>302478</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>136544</v>
+      </c>
+      <c r="C5" s="4">
+        <v>136600</v>
+      </c>
+      <c r="D5" s="4">
+        <v>207417</v>
+      </c>
+      <c r="E5" s="4">
+        <v>219981</v>
+      </c>
+      <c r="F5" s="4">
+        <v>164999</v>
+      </c>
+      <c r="G5" s="4">
+        <v>134319</v>
+      </c>
+      <c r="H5" s="4">
+        <v>137889</v>
+      </c>
+      <c r="I5" s="4">
+        <v>216376</v>
+      </c>
+      <c r="J5" s="4">
+        <v>238740</v>
+      </c>
+      <c r="K5" s="4">
+        <v>266083</v>
+      </c>
+      <c r="L5" s="4">
+        <v>283503</v>
+      </c>
+      <c r="M5" s="4">
+        <v>303065</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>136544</v>
+      </c>
+      <c r="C6" s="4">
+        <v>136600</v>
+      </c>
+      <c r="D6" s="4">
+        <v>207417</v>
+      </c>
+      <c r="E6" s="4">
+        <v>219981</v>
+      </c>
+      <c r="F6" s="4">
+        <v>164999</v>
+      </c>
+      <c r="G6" s="4">
+        <v>133551</v>
+      </c>
+      <c r="H6" s="4">
+        <v>138871</v>
+      </c>
+      <c r="I6" s="4">
+        <v>215298</v>
+      </c>
+      <c r="J6" s="4">
+        <v>238740</v>
+      </c>
+      <c r="K6" s="4">
+        <v>264686</v>
+      </c>
+      <c r="L6" s="4">
+        <v>286293</v>
+      </c>
+      <c r="M6" s="4">
+        <v>303065</v>
       </c>
     </row>
   </sheetData>
@@ -2359,9 +3630,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:I1"/>
@@ -2460,14 +3731,72 @@
         <v>420147</v>
       </c>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>339925</v>
+      </c>
+      <c r="C5" s="4">
+        <v>387990</v>
+      </c>
+      <c r="D5" s="4">
+        <v>481965</v>
+      </c>
+      <c r="E5" s="4">
+        <v>205434</v>
+      </c>
+      <c r="F5" s="4">
+        <v>248025</v>
+      </c>
+      <c r="G5" s="4">
+        <v>421096</v>
+      </c>
+      <c r="H5" s="4">
+        <v>413255</v>
+      </c>
+      <c r="I5" s="4">
+        <v>419480</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>339925</v>
+      </c>
+      <c r="C6" s="4">
+        <v>387990</v>
+      </c>
+      <c r="D6" s="4">
+        <v>480730</v>
+      </c>
+      <c r="E6" s="4">
+        <v>206117</v>
+      </c>
+      <c r="F6" s="4">
+        <v>249078</v>
+      </c>
+      <c r="G6" s="4">
+        <v>420471</v>
+      </c>
+      <c r="H6" s="4">
+        <v>420622</v>
+      </c>
+      <c r="I6" s="4">
+        <v>419314</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:G3"/>
@@ -2548,14 +3877,60 @@
         <v>123635</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>126618</v>
+      </c>
+      <c r="C5" s="4">
+        <v>118806</v>
+      </c>
+      <c r="D5" s="4">
+        <v>122637</v>
+      </c>
+      <c r="E5" s="4">
+        <v>127181</v>
+      </c>
+      <c r="F5" s="4">
+        <v>121452</v>
+      </c>
+      <c r="G5" s="4">
+        <v>123635</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>126475</v>
+      </c>
+      <c r="C6" s="4">
+        <v>118690</v>
+      </c>
+      <c r="D6" s="4">
+        <v>122506</v>
+      </c>
+      <c r="E6" s="4">
+        <v>126987</v>
+      </c>
+      <c r="F6" s="4">
+        <v>121279</v>
+      </c>
+      <c r="G6" s="4">
+        <v>123635</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:D3"/>
@@ -2609,14 +3984,42 @@
         <v>234171</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>209204</v>
+      </c>
+      <c r="C5" s="4">
+        <v>217322</v>
+      </c>
+      <c r="D5" s="4">
+        <v>233772</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>209090</v>
+      </c>
+      <c r="C6" s="4">
+        <v>217265</v>
+      </c>
+      <c r="D6" s="4">
+        <v>235338</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M1" sqref="A1:M1"/>
@@ -2752,14 +4155,96 @@
         <v>113107</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>17297</v>
+      </c>
+      <c r="C5" s="4">
+        <v>19121</v>
+      </c>
+      <c r="D5" s="4">
+        <v>24145</v>
+      </c>
+      <c r="E5" s="4">
+        <v>25428</v>
+      </c>
+      <c r="F5" s="4">
+        <v>27868</v>
+      </c>
+      <c r="G5" s="4">
+        <v>40049</v>
+      </c>
+      <c r="H5" s="4">
+        <v>53070</v>
+      </c>
+      <c r="I5" s="4">
+        <v>59963</v>
+      </c>
+      <c r="J5" s="4">
+        <v>77358</v>
+      </c>
+      <c r="K5" s="4">
+        <v>87130</v>
+      </c>
+      <c r="L5" s="4">
+        <v>103323</v>
+      </c>
+      <c r="M5" s="4">
+        <v>113501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>17041</v>
+      </c>
+      <c r="C6" s="4">
+        <v>19094</v>
+      </c>
+      <c r="D6" s="4">
+        <v>24156</v>
+      </c>
+      <c r="E6" s="4">
+        <v>25435</v>
+      </c>
+      <c r="F6" s="4">
+        <v>27923</v>
+      </c>
+      <c r="G6" s="4">
+        <v>40506</v>
+      </c>
+      <c r="H6" s="4">
+        <v>52794</v>
+      </c>
+      <c r="I6" s="4">
+        <v>59933</v>
+      </c>
+      <c r="J6" s="4">
+        <v>77457</v>
+      </c>
+      <c r="K6" s="4">
+        <v>87170</v>
+      </c>
+      <c r="L6" s="4">
+        <v>102937</v>
+      </c>
+      <c r="M6" s="4">
+        <v>113541</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:L3"/>
@@ -2885,14 +4370,318 @@
         <v>77719</v>
       </c>
     </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>20437</v>
+      </c>
+      <c r="C5" s="4">
+        <v>22175</v>
+      </c>
+      <c r="D5" s="4">
+        <v>24852</v>
+      </c>
+      <c r="E5" s="4">
+        <v>28980</v>
+      </c>
+      <c r="F5" s="4">
+        <v>32382</v>
+      </c>
+      <c r="G5" s="4">
+        <v>39300</v>
+      </c>
+      <c r="H5" s="4">
+        <v>45579</v>
+      </c>
+      <c r="I5" s="4">
+        <v>54375</v>
+      </c>
+      <c r="J5" s="4">
+        <v>59082</v>
+      </c>
+      <c r="K5" s="4">
+        <v>68362</v>
+      </c>
+      <c r="L5" s="4">
+        <v>77843</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>20407</v>
+      </c>
+      <c r="C6" s="4">
+        <v>22092</v>
+      </c>
+      <c r="D6" s="4">
+        <v>24804</v>
+      </c>
+      <c r="E6" s="4">
+        <v>29026</v>
+      </c>
+      <c r="F6" s="4">
+        <v>32285</v>
+      </c>
+      <c r="G6" s="4">
+        <v>39431</v>
+      </c>
+      <c r="H6" s="4">
+        <v>45459</v>
+      </c>
+      <c r="I6" s="4">
+        <v>54205</v>
+      </c>
+      <c r="J6" s="4">
+        <v>58894</v>
+      </c>
+      <c r="K6" s="4">
+        <v>68281</v>
+      </c>
+      <c r="L6" s="4">
+        <v>77668</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5">
+        <v>2007</v>
+      </c>
+      <c r="C1" s="5">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>27237</v>
+      </c>
+      <c r="C3" s="4">
+        <v>41975</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>27237</v>
+      </c>
+      <c r="C4" s="4">
+        <v>40262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>27237</v>
+      </c>
+      <c r="C5" s="4">
+        <v>40262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>26544</v>
+      </c>
+      <c r="C6" s="4">
+        <v>40062</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6">
+        <v>2020</v>
+      </c>
+      <c r="C1" s="6">
+        <v>2021</v>
+      </c>
+      <c r="D1" s="6">
+        <v>2022</v>
+      </c>
+      <c r="E1" s="6">
+        <v>2023</v>
+      </c>
+      <c r="F1" s="6">
+        <v>2024</v>
+      </c>
+      <c r="G1" s="6">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>90504</v>
+      </c>
+      <c r="C6" s="4">
+        <v>98670</v>
+      </c>
+      <c r="D6" s="4">
+        <v>110213</v>
+      </c>
+      <c r="E6" s="4">
+        <v>144656</v>
+      </c>
+      <c r="F6" s="4">
+        <v>161100</v>
+      </c>
+      <c r="G6" s="4">
+        <v>203928</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6">
+        <v>2013</v>
+      </c>
+      <c r="C1" s="6">
+        <v>2014</v>
+      </c>
+      <c r="D1" s="6">
+        <v>2015</v>
+      </c>
+      <c r="E1" s="6">
+        <v>2016</v>
+      </c>
+      <c r="F1" s="6">
+        <v>2017</v>
+      </c>
+      <c r="G1" s="6">
+        <v>2018</v>
+      </c>
+      <c r="H1" s="6">
+        <v>2019</v>
+      </c>
+      <c r="I1" s="6">
+        <v>2020</v>
+      </c>
+      <c r="J1" s="6">
+        <v>2022</v>
+      </c>
+      <c r="K1" s="6">
+        <v>2023</v>
+      </c>
+      <c r="L1" s="6">
+        <v>2024</v>
+      </c>
+      <c r="M1" s="6">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>14992</v>
+      </c>
+      <c r="C6" s="4">
+        <v>15401</v>
+      </c>
+      <c r="D6" s="4">
+        <v>16539</v>
+      </c>
+      <c r="E6" s="4">
+        <v>17983</v>
+      </c>
+      <c r="F6" s="4">
+        <v>20979</v>
+      </c>
+      <c r="G6" s="4">
+        <v>21977</v>
+      </c>
+      <c r="H6" s="4">
+        <v>23436</v>
+      </c>
+      <c r="I6" s="4">
+        <v>23369</v>
+      </c>
+      <c r="J6" s="4">
+        <v>27508</v>
+      </c>
+      <c r="K6" s="4">
+        <v>27834</v>
+      </c>
+      <c r="L6" s="4">
+        <v>32788</v>
+      </c>
+      <c r="M6" s="4">
+        <v>37374</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="A3:H3"/>
@@ -2982,16 +4771,68 @@
         <v>45196</v>
       </c>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>22761</v>
+      </c>
+      <c r="C5" s="4">
+        <v>22069</v>
+      </c>
+      <c r="D5" s="4">
+        <v>24633</v>
+      </c>
+      <c r="E5" s="4">
+        <v>26636</v>
+      </c>
+      <c r="F5" s="4">
+        <v>27945</v>
+      </c>
+      <c r="G5" s="4">
+        <v>31861</v>
+      </c>
+      <c r="H5" s="4">
+        <v>45152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>22823</v>
+      </c>
+      <c r="C6" s="4">
+        <v>22085</v>
+      </c>
+      <c r="D6" s="4">
+        <v>24700</v>
+      </c>
+      <c r="E6" s="4">
+        <v>26617</v>
+      </c>
+      <c r="F6" s="4">
+        <v>27699</v>
+      </c>
+      <c r="G6" s="4">
+        <v>31729</v>
+      </c>
+      <c r="H6" s="4">
+        <v>45132</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -3052,56 +4893,208 @@
         <v>39525</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>29863</v>
+      </c>
+      <c r="C5" s="4">
+        <v>33005</v>
+      </c>
+      <c r="D5" s="4">
+        <v>33156</v>
+      </c>
+      <c r="E5" s="4">
+        <v>39464</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>29908</v>
+      </c>
+      <c r="C6" s="4">
+        <v>33108</v>
+      </c>
+      <c r="D6" s="4">
+        <v>32914</v>
+      </c>
+      <c r="E6" s="4">
+        <v>39464</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C4"/>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6">
+        <v>2024</v>
+      </c>
+      <c r="C1" s="6">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>87768</v>
+      </c>
+      <c r="C6" s="4">
+        <v>80300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6">
+        <v>2020</v>
+      </c>
+      <c r="C1" s="6">
+        <v>2021</v>
+      </c>
+      <c r="D1" s="6">
+        <v>2022</v>
+      </c>
+      <c r="E1" s="6">
+        <v>2023</v>
+      </c>
+      <c r="F1" s="6">
+        <v>2024</v>
+      </c>
+      <c r="G1" s="6">
+        <v>2025</v>
+      </c>
+      <c r="H1" s="6">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>26077</v>
+      </c>
+      <c r="C6" s="4">
+        <v>26951</v>
+      </c>
+      <c r="D6" s="4">
+        <v>28859</v>
+      </c>
+      <c r="E6" s="4">
+        <v>32240</v>
+      </c>
+      <c r="F6" s="4">
+        <v>35795</v>
+      </c>
+      <c r="G6" s="4">
+        <v>40201</v>
+      </c>
+      <c r="H6" s="4">
+        <v>58944</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5">
-        <v>2007</v>
-      </c>
-      <c r="C1" s="5">
-        <v>2008</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4">
-        <v>27237</v>
-      </c>
-      <c r="C3" s="4">
-        <v>41975</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4">
-        <v>27237</v>
-      </c>
-      <c r="C4" s="4">
-        <v>40262</v>
+      <c r="B1" s="6">
+        <v>2020</v>
+      </c>
+      <c r="C1" s="6">
+        <v>2021</v>
+      </c>
+      <c r="D1" s="6">
+        <v>2022</v>
+      </c>
+      <c r="E1" s="6">
+        <v>2023</v>
+      </c>
+      <c r="F1" s="6">
+        <v>2024</v>
+      </c>
+      <c r="G1" s="6">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>90504</v>
+      </c>
+      <c r="C6" s="4">
+        <v>98670</v>
+      </c>
+      <c r="D6" s="4">
+        <v>110213</v>
+      </c>
+      <c r="E6" s="4">
+        <v>144656</v>
+      </c>
+      <c r="F6" s="4">
+        <v>161100</v>
+      </c>
+      <c r="G6" s="4">
+        <v>203928</v>
       </c>
     </row>
   </sheetData>
@@ -3111,7 +5104,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E11:E12"/>
@@ -3229,6 +5222,76 @@
         <v>145919</v>
       </c>
     </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>37982</v>
+      </c>
+      <c r="C5" s="4">
+        <v>45652</v>
+      </c>
+      <c r="D5" s="4">
+        <v>42735</v>
+      </c>
+      <c r="E5" s="4">
+        <v>58790</v>
+      </c>
+      <c r="F5" s="4">
+        <v>58818</v>
+      </c>
+      <c r="G5" s="4">
+        <v>80055</v>
+      </c>
+      <c r="H5" s="4">
+        <v>92377</v>
+      </c>
+      <c r="I5" s="4">
+        <v>101511</v>
+      </c>
+      <c r="J5" s="4">
+        <v>134745</v>
+      </c>
+      <c r="K5" s="4">
+        <v>145777</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>37816</v>
+      </c>
+      <c r="C6" s="4">
+        <v>45556</v>
+      </c>
+      <c r="D6" s="4">
+        <v>42687</v>
+      </c>
+      <c r="E6" s="4">
+        <v>58930</v>
+      </c>
+      <c r="F6" s="4">
+        <v>58651</v>
+      </c>
+      <c r="G6" s="4">
+        <v>79790</v>
+      </c>
+      <c r="H6" s="4">
+        <v>92204</v>
+      </c>
+      <c r="I6" s="4">
+        <v>101419</v>
+      </c>
+      <c r="J6" s="4">
+        <v>134348</v>
+      </c>
+      <c r="K6" s="4">
+        <v>145703</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3236,16 +5299,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3292,7 +5356,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3">
         <v>8974</v>
@@ -3407,6 +5471,85 @@
         <v>44530</v>
       </c>
       <c r="M4" s="4">
+        <v>53140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>8647</v>
+      </c>
+      <c r="C5" s="4">
+        <v>9225</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E5" s="4">
+        <v>17444</v>
+      </c>
+      <c r="F5" s="4">
+        <v>20700</v>
+      </c>
+      <c r="G5" s="4">
+        <v>19883</v>
+      </c>
+      <c r="H5" s="4">
+        <v>24764</v>
+      </c>
+      <c r="I5" s="4">
+        <v>28913</v>
+      </c>
+      <c r="J5" s="4">
+        <v>36301</v>
+      </c>
+      <c r="K5" s="4">
+        <v>45345</v>
+      </c>
+      <c r="L5" s="4">
+        <v>44783</v>
+      </c>
+      <c r="M5" s="4">
+        <v>53140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>8647</v>
+      </c>
+      <c r="C6" s="4">
+        <v>9225</v>
+      </c>
+      <c r="E6" s="4">
+        <v>17444</v>
+      </c>
+      <c r="F6" s="4">
+        <v>19300</v>
+      </c>
+      <c r="G6" s="4">
+        <v>20216</v>
+      </c>
+      <c r="H6" s="4">
+        <v>25669</v>
+      </c>
+      <c r="I6" s="4">
+        <v>28913</v>
+      </c>
+      <c r="J6" s="4">
+        <v>37790</v>
+      </c>
+      <c r="K6" s="4">
+        <v>46129</v>
+      </c>
+      <c r="L6" s="4">
+        <v>44575</v>
+      </c>
+      <c r="M6" s="4">
         <v>53140</v>
       </c>
     </row>
@@ -3416,8 +5559,55 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6">
+        <v>2022</v>
+      </c>
+      <c r="C1" s="6">
+        <v>2023</v>
+      </c>
+      <c r="D1" s="6">
+        <v>2024</v>
+      </c>
+      <c r="E1" s="6">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>70142</v>
+      </c>
+      <c r="C6" s="4">
+        <v>81400</v>
+      </c>
+      <c r="D6" s="4">
+        <v>98351</v>
+      </c>
+      <c r="E6" s="4">
+        <v>173219</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:M3"/>
@@ -3552,14 +5742,96 @@
         <v>52363</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>45148</v>
+      </c>
+      <c r="C5" s="4">
+        <v>36936</v>
+      </c>
+      <c r="D5" s="4">
+        <v>38435</v>
+      </c>
+      <c r="E5" s="4">
+        <v>29963</v>
+      </c>
+      <c r="F5" s="4">
+        <v>36970</v>
+      </c>
+      <c r="G5" s="4">
+        <v>40006</v>
+      </c>
+      <c r="H5" s="4">
+        <v>34946</v>
+      </c>
+      <c r="I5" s="4">
+        <v>31439</v>
+      </c>
+      <c r="J5" s="4">
+        <v>34512</v>
+      </c>
+      <c r="K5" s="4">
+        <v>43041</v>
+      </c>
+      <c r="L5" s="4">
+        <v>50047</v>
+      </c>
+      <c r="M5" s="4">
+        <v>52283</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>46266</v>
+      </c>
+      <c r="C6" s="4">
+        <v>36936</v>
+      </c>
+      <c r="D6" s="4">
+        <v>38902</v>
+      </c>
+      <c r="E6" s="4">
+        <v>30024</v>
+      </c>
+      <c r="F6" s="4">
+        <v>37583</v>
+      </c>
+      <c r="G6" s="4">
+        <v>40006</v>
+      </c>
+      <c r="H6" s="4">
+        <v>35057</v>
+      </c>
+      <c r="I6" s="4">
+        <v>31586</v>
+      </c>
+      <c r="J6" s="4">
+        <v>34313</v>
+      </c>
+      <c r="K6" s="4">
+        <v>44026</v>
+      </c>
+      <c r="L6" s="4">
+        <v>50125</v>
+      </c>
+      <c r="M6" s="4">
+        <v>50445</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
@@ -3615,7 +5887,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3">
         <v>30730</v>
@@ -3736,147 +6008,86 @@
         <v>128435</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:M4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39:D40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5">
-        <v>2007</v>
-      </c>
-      <c r="C1" s="5">
-        <v>2014</v>
-      </c>
-      <c r="D1" s="5">
-        <v>2015</v>
-      </c>
-      <c r="E1" s="5">
-        <v>2016</v>
-      </c>
-      <c r="F1" s="5">
-        <v>2017</v>
-      </c>
-      <c r="G1" s="5">
-        <v>2019</v>
-      </c>
-      <c r="H1" s="5">
-        <v>2020</v>
-      </c>
-      <c r="I1" s="5">
-        <v>2021</v>
-      </c>
-      <c r="J1" s="5">
-        <v>2022</v>
-      </c>
-      <c r="K1" s="5">
-        <v>2023</v>
-      </c>
-      <c r="L1" s="5">
-        <v>2024</v>
-      </c>
-      <c r="M1" s="5">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4">
-        <v>35555</v>
-      </c>
-      <c r="C3" s="4">
-        <v>41770</v>
-      </c>
-      <c r="D3" s="4">
-        <v>50691</v>
-      </c>
-      <c r="E3" s="4">
-        <v>57343</v>
-      </c>
-      <c r="F3" s="4">
-        <v>56857</v>
-      </c>
-      <c r="G3" s="4">
-        <v>77363</v>
-      </c>
-      <c r="H3" s="4">
-        <v>67876</v>
-      </c>
-      <c r="I3" s="4">
-        <v>68121</v>
-      </c>
-      <c r="J3" s="4">
-        <v>70376</v>
-      </c>
-      <c r="K3" s="4">
-        <v>82645</v>
-      </c>
-      <c r="L3" s="4">
-        <v>90514</v>
-      </c>
-      <c r="M3" s="4">
-        <v>107589</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4">
-        <v>35428</v>
-      </c>
-      <c r="C4" s="4">
-        <v>41902</v>
-      </c>
-      <c r="D4" s="4">
-        <v>50744</v>
-      </c>
-      <c r="E4" s="4">
-        <v>57411</v>
-      </c>
-      <c r="F4" s="4">
-        <v>56616</v>
-      </c>
-      <c r="G4" s="4">
-        <v>77738</v>
-      </c>
-      <c r="H4" s="4">
-        <v>67932</v>
-      </c>
-      <c r="I4" s="4">
-        <v>68118</v>
-      </c>
-      <c r="J4" s="4">
-        <v>70225</v>
-      </c>
-      <c r="K4" s="4">
-        <v>82788</v>
-      </c>
-      <c r="L4" s="4">
-        <v>90339</v>
-      </c>
-      <c r="M4" s="4">
-        <v>107625</v>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>30851</v>
+      </c>
+      <c r="C5" s="4">
+        <v>29456</v>
+      </c>
+      <c r="D5" s="4">
+        <v>33471</v>
+      </c>
+      <c r="E5" s="4">
+        <v>38705</v>
+      </c>
+      <c r="F5" s="4">
+        <v>52782</v>
+      </c>
+      <c r="G5" s="4">
+        <v>56946</v>
+      </c>
+      <c r="H5" s="4">
+        <v>64586</v>
+      </c>
+      <c r="I5" s="4">
+        <v>76241</v>
+      </c>
+      <c r="J5" s="4">
+        <v>95648</v>
+      </c>
+      <c r="K5" s="4">
+        <v>97464</v>
+      </c>
+      <c r="L5" s="4">
+        <v>132075</v>
+      </c>
+      <c r="M5" s="4">
+        <v>128504</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>30506</v>
+      </c>
+      <c r="C6" s="4">
+        <v>29738</v>
+      </c>
+      <c r="D6" s="4">
+        <v>33338</v>
+      </c>
+      <c r="E6" s="4">
+        <v>39560</v>
+      </c>
+      <c r="F6" s="4">
+        <v>52814</v>
+      </c>
+      <c r="G6" s="4">
+        <v>56629</v>
+      </c>
+      <c r="H6" s="4">
+        <v>64398</v>
+      </c>
+      <c r="I6" s="4">
+        <v>76102</v>
+      </c>
+      <c r="J6" s="4">
+        <v>97282</v>
+      </c>
+      <c r="K6" s="4">
+        <v>97912</v>
+      </c>
+      <c r="L6" s="4">
+        <v>132097</v>
+      </c>
+      <c r="M6" s="4">
+        <v>128498</v>
       </c>
     </row>
   </sheetData>
@@ -3885,86 +6096,93 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5">
-        <v>2010</v>
-      </c>
-      <c r="C1" s="5">
-        <v>2011</v>
-      </c>
-      <c r="D1" s="5">
-        <v>2012</v>
-      </c>
-      <c r="E1" s="5">
-        <v>2013</v>
-      </c>
-      <c r="F1" s="5">
+      <c r="B1" s="6">
+        <v>2003</v>
+      </c>
+      <c r="C1" s="6">
+        <v>2005</v>
+      </c>
+      <c r="D1" s="6">
         <v>2014</v>
       </c>
-      <c r="G1" s="5">
+      <c r="E1" s="6">
         <v>2015</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4">
-        <v>194782</v>
-      </c>
-      <c r="C3" s="4">
-        <v>201635</v>
-      </c>
-      <c r="D3" s="4">
-        <v>204811</v>
-      </c>
-      <c r="E3" s="4">
-        <v>213776</v>
-      </c>
-      <c r="F3" s="4">
-        <v>249238</v>
-      </c>
-      <c r="G3" s="4">
-        <v>221576</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4">
-        <v>195060</v>
-      </c>
-      <c r="C4" s="4">
-        <v>204060</v>
-      </c>
-      <c r="D4" s="4">
-        <v>204478</v>
-      </c>
-      <c r="E4" s="4">
-        <v>213776</v>
-      </c>
-      <c r="F4" s="4">
-        <v>249238</v>
-      </c>
-      <c r="G4" s="4">
-        <v>221576</v>
+      <c r="F1" s="6">
+        <v>2017</v>
+      </c>
+      <c r="G1" s="6">
+        <v>2019</v>
+      </c>
+      <c r="H1" s="6">
+        <v>2020</v>
+      </c>
+      <c r="I1" s="6">
+        <v>2021</v>
+      </c>
+      <c r="J1" s="6">
+        <v>2022</v>
+      </c>
+      <c r="K1" s="6">
+        <v>2023</v>
+      </c>
+      <c r="L1" s="6">
+        <v>2024</v>
+      </c>
+      <c r="M1" s="6">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>33000</v>
+      </c>
+      <c r="C6" s="4">
+        <v>22400</v>
+      </c>
+      <c r="D6" s="4">
+        <v>36246</v>
+      </c>
+      <c r="E6" s="4">
+        <v>55112</v>
+      </c>
+      <c r="F6" s="4">
+        <v>47966</v>
+      </c>
+      <c r="G6" s="4">
+        <v>66280</v>
+      </c>
+      <c r="H6" s="4">
+        <v>69325</v>
+      </c>
+      <c r="I6" s="4">
+        <v>71248</v>
+      </c>
+      <c r="J6" s="4">
+        <v>80162</v>
+      </c>
+      <c r="K6" s="4">
+        <v>74222</v>
+      </c>
+      <c r="L6" s="4">
+        <v>82648</v>
+      </c>
+      <c r="M6" s="4">
+        <v>108247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>